<commit_message>
Added page to sketch out EPFImporter, EPFIngester, EPFParser and EPFDbUtil interfaces
git-svn-id: http://www.spazzdev.com/spazz_serverj/trunk@63 4839df1b-77b6-4aaf-b387-209ca36962b6
</commit_message>
<xml_diff>
--- a/spazzmania-cron/notes/SynchronizedCron.xlsx
+++ b/spazzmania-cron/notes/SynchronizedCron.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="19035" windowHeight="8445" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="19035" windowHeight="8445" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="EPFImporter" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="199">
   <si>
     <t>SynchronizedJob</t>
   </si>
@@ -538,6 +539,81 @@
   </si>
   <si>
     <t>Schedule the Job</t>
+  </si>
+  <si>
+    <t>EPFImporter Interface Definitions</t>
+  </si>
+  <si>
+    <t>EPFImporter</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Load Configuration Files</t>
+  </si>
+  <si>
+    <t>Load Command Line Parameters</t>
+  </si>
+  <si>
+    <t>Import Directory</t>
+  </si>
+  <si>
+    <t>Import Files</t>
+  </si>
+  <si>
+    <t>Import Whitelist</t>
+  </si>
+  <si>
+    <t>Import Blacklist</t>
+  </si>
+  <si>
+    <t>For each file to import</t>
+  </si>
+  <si>
+    <t>Load Thread Pool Maximum</t>
+  </si>
+  <si>
+    <t>EPFIngester</t>
+  </si>
+  <si>
+    <t>ExecutionQueue.add(new EPFIngester(importFile))</t>
+  </si>
+  <si>
+    <t>new EPFParser(new EPFFileReader(importFile))</t>
+  </si>
+  <si>
+    <t>parseTableName</t>
+  </si>
+  <si>
+    <t>parseColumnsAndTypes</t>
+  </si>
+  <si>
+    <t>parsePrimaryKey</t>
+  </si>
+  <si>
+    <t>seekRecord()</t>
+  </si>
+  <si>
+    <t>totalRecords()</t>
+  </si>
+  <si>
+    <t>nextRecord()</t>
+  </si>
+  <si>
+    <t>EPFDbUtil</t>
+  </si>
+  <si>
+    <t>initTable(tableName,importType,totalRecords)</t>
+  </si>
+  <si>
+    <t>createTable(tableName,columnsAndTypes,primaryKeys)</t>
+  </si>
+  <si>
+    <t>insertRow(List&lt;String&gt; values)</t>
+  </si>
+  <si>
+    <t>finalizeTable()</t>
   </si>
 </sst>
 </file>
@@ -1405,7 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
@@ -1938,4 +2014,144 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the design notes
git-svn-id: http://www.spazzdev.com/spazz_serverj/trunk@72 4839df1b-77b6-4aaf-b387-209ca36962b6
</commit_message>
<xml_diff>
--- a/spazzmania-cron/notes/SynchronizedCron.xlsx
+++ b/spazzmania-cron/notes/SynchronizedCron.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="19035" windowHeight="8445" activeTab="3"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="216">
   <si>
     <t>SynchronizedJob</t>
   </si>
@@ -617,6 +617,54 @@
   </si>
   <si>
     <t>EPFParser</t>
+  </si>
+  <si>
+    <t>ConnectionPool</t>
+  </si>
+  <si>
+    <t>EPFIngesterQueue</t>
+  </si>
+  <si>
+    <t>add(fileName)</t>
+  </si>
+  <si>
+    <t>setQueueSize()</t>
+  </si>
+  <si>
+    <t>ExecutorService executor = Executors.newFixedThreadPool(NTHREDS);</t>
+  </si>
+  <si>
+    <t>This is originally intended to use the Executors.newFixedTheadPool() logic</t>
+  </si>
+  <si>
+    <t>This could also be implemented using Quartz scheduler threads</t>
+  </si>
+  <si>
+    <t>The fileName is all an EPFIngester needs to process</t>
+  </si>
+  <si>
+    <t>And a connection Pool</t>
+  </si>
+  <si>
+    <t>Use Apache's org.apache.commons.dbcp</t>
+  </si>
+  <si>
+    <t>This allows the designation of the minimum and maximum number of concurrent connections.</t>
+  </si>
+  <si>
+    <t>It also allows for virtual opening and closing of connections where "closing" merely returns the connection to the pool.</t>
+  </si>
+  <si>
+    <t>This also means that the underlying connector needs to open and close connections whenever it performs a single SQL statement or a small block of statements</t>
+  </si>
+  <si>
+    <t>setConnectionPool()</t>
+  </si>
+  <si>
+    <t>isTableExists()</t>
+  </si>
+  <si>
+    <t>getTableColumnCount()</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1533,7 @@
   <dimension ref="A2:E130"/>
   <sheetViews>
     <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,10 +2069,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,72 +2139,146 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>201</v>
+      </c>
+      <c r="I23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>213</v>
+      </c>
+      <c r="I25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving the model design to UML
git-svn-id: http://www.spazzdev.com/spazz_serverj/trunk@101 4839df1b-77b6-4aaf-b387-209ca36962b6
</commit_message>
<xml_diff>
--- a/spazzmania-cron/notes/SynchronizedCron.xlsx
+++ b/spazzmania-cron/notes/SynchronizedCron.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="EPFImporter" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="EPFImporter" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="232">
   <si>
     <t>SynchronizedJob</t>
   </si>
@@ -98,7 +97,7 @@
     <t>SyncWaitJobErrorHandling</t>
   </si>
   <si>
-    <t>The same as SyncWaitForJobGroup </t>
+    <t>The same as SyncWaitForJobGroup</t>
   </si>
   <si>
     <t>WorkFlow</t>
@@ -275,7 +274,7 @@
     <t>Job1 - storeDurably()</t>
   </si>
   <si>
-    <t>JobListener - </t>
+    <t>JobListener -</t>
   </si>
   <si>
     <t>WorkflowTask</t>
@@ -383,7 +382,7 @@
     <t>Step 2 - Load all Jobs to be executed into the scheduler with storeDurably() set to true</t>
   </si>
   <si>
-    <t>Step 3 - Load all Dependencies as WorkflowTask listeners.  </t>
+    <t>Step 3 - Load all Dependencies as WorkflowTask listeners.</t>
   </si>
   <si>
     <t>WorkflowTasks with no depenencies are loaded last (they execute immediately)</t>
@@ -506,7 +505,7 @@
     <t>This is the starship enterprise</t>
   </si>
   <si>
-    <t>Whose continuing mission </t>
+    <t>Whose continuing mission</t>
   </si>
   <si>
     <t>is to seek out new life and new civilizations</t>
@@ -569,7 +568,7 @@
     <t>Load Thread Pool Maximum</t>
   </si>
   <si>
-    <t>Loads the configuration </t>
+    <t>Loads the configuration</t>
   </si>
   <si>
     <t>Launches EPFImportManager handing over the DBConfig and EPFConfig info</t>
@@ -593,9 +592,6 @@
     <t>For each file to import</t>
   </si>
   <si>
-    <t>ExecutionQueue.add(new EPFIngester(connector,importFile))</t>
-  </si>
-  <si>
     <t>ConnectionPool</t>
   </si>
   <si>
@@ -638,12 +634,6 @@
     <t>And a connection Pool</t>
   </si>
   <si>
-    <t>EPFIngester</t>
-  </si>
-  <si>
-    <t>new EPFParser(new EPFFileReader(importFile))</t>
-  </si>
-  <si>
     <t>EPFParser</t>
   </si>
   <si>
@@ -684,45 +674,73 @@
   </si>
   <si>
     <t>isTableExists()</t>
+  </si>
+  <si>
+    <t>EPFImportTask</t>
+  </si>
+  <si>
+    <t>run()</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>fileNamePath</t>
+  </si>
+  <si>
+    <t>EFPConfig config = EPFImportManager.getInstance().getConfig();</t>
+  </si>
+  <si>
+    <t>Instantiate</t>
+  </si>
+  <si>
+    <t>BoneCP connector = EPFImportManager.getInstance().getConnector();</t>
+  </si>
+  <si>
+    <t>new EPFParser (fileReader, rowDelimiter, fieldDelimiter)</t>
+  </si>
+  <si>
+    <t>new EPFFileReader(fileNamePath)</t>
+  </si>
+  <si>
+    <t>EPFDbConfig</t>
+  </si>
+  <si>
+    <t>EPFConfig</t>
+  </si>
+  <si>
+    <t>getEPFFileParser(fileNameAndPath);</t>
+  </si>
+  <si>
+    <t>ExecutionQueue.add(new EPFImportTask(connector,parser))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
       <family val="2"/>
-      <i val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -734,7 +752,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -742,1411 +760,1693 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B18" activeCellId="0" pane="topLeft" sqref="B18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
-      <c r="B2" s="0" t="s">
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
-      <c r="B4" s="0" t="s">
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
-      <c r="B5" s="0" t="s">
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
-      <c r="B8" s="0" t="s">
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
-      <c r="B9" s="0" t="s">
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="B11" s="0" t="s">
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
-      <c r="B14" s="0" t="s">
+    <row r="14" spans="1:2">
+      <c r="B14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
-      <c r="B15" s="0" t="s">
+    <row r="15" spans="1:2">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="16">
-      <c r="B16" s="0" t="s">
+    <row r="16" spans="1:2">
+      <c r="B16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
-      <c r="B17" s="0" t="s">
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="18">
-      <c r="B18" s="0" t="s">
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="20">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="21">
-      <c r="B21" s="0" t="s">
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="22">
-      <c r="B22" s="0" t="s">
+    <row r="22" spans="1:3">
+      <c r="B22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="23">
-      <c r="B23" s="0" t="s">
+    <row r="23" spans="1:3">
+      <c r="B23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
-      <c r="C24" s="0" t="s">
+    <row r="24" spans="1:3">
+      <c r="C24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
-      <c r="C25" s="0" t="s">
+    <row r="25" spans="1:3">
+      <c r="C25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="26">
-      <c r="C26" s="0" t="s">
+    <row r="26" spans="1:3">
+      <c r="C26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="28">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="29">
-      <c r="B29" s="0" t="s">
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="30">
-      <c r="B30" s="0" t="s">
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="31">
-      <c r="B31" s="0" t="s">
+    <row r="31" spans="1:3">
+      <c r="B31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="32">
-      <c r="B32" s="0" t="s">
+    <row r="32" spans="1:3">
+      <c r="B32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="33">
-      <c r="C33" s="0" t="s">
+    <row r="33" spans="3:3">
+      <c r="C33" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A2:G83"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E16" activeCellId="0" pane="topLeft" sqref="E16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4705882352941"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.71372549019608"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="10.42578125"/>
+    <col min="3" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
-      <c r="B3" s="0" t="s">
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
-      <c r="B4" s="0" t="s">
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
-      <c r="B5" s="0" t="s">
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
-      <c r="B6" s="0" t="s">
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
-      <c r="B7" s="0" t="s">
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="B11" s="0" t="s">
+    <row r="11" spans="1:7">
+      <c r="B11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
-      <c r="C12" s="0" t="s">
+    <row r="12" spans="1:7">
+      <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
-      <c r="C13" s="0" t="s">
+    <row r="13" spans="1:7">
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
-      <c r="C14" s="0" t="s">
+    <row r="14" spans="1:7">
+      <c r="C14" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="16">
-      <c r="B16" s="0" t="s">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
-      <c r="C17" s="0" t="s">
+    <row r="17" spans="1:6">
+      <c r="C17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="18">
-      <c r="D18" s="0" t="s">
+    <row r="18" spans="1:6">
+      <c r="D18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="19">
-      <c r="E19" s="0" t="s">
+    <row r="19" spans="1:6">
+      <c r="E19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="20">
-      <c r="F20" s="0" t="s">
+    <row r="20" spans="1:6">
+      <c r="F20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="21">
-      <c r="F21" s="0" t="s">
+    <row r="21" spans="1:6">
+      <c r="F21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="22">
-      <c r="E22" s="0" t="s">
+    <row r="22" spans="1:6">
+      <c r="E22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="23">
-      <c r="F23" s="0" t="s">
+    <row r="23" spans="1:6">
+      <c r="F23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
-      <c r="F24" s="0" t="s">
+    <row r="24" spans="1:6">
+      <c r="F24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
-      <c r="D25" s="0" t="s">
+    <row r="25" spans="1:6">
+      <c r="D25" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="28">
-      <c r="B28" s="0" t="s">
+    <row r="28" spans="1:6">
+      <c r="B28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="29">
-      <c r="B29" s="0" t="s">
+    <row r="29" spans="1:6">
+      <c r="B29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="30">
-      <c r="B30" s="0" t="s">
+    <row r="30" spans="1:6">
+      <c r="B30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="32">
-      <c r="B32" s="0" t="s">
+    <row r="32" spans="1:6">
+      <c r="B32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="33">
-      <c r="B33" s="0" t="s">
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="34">
-      <c r="B34" s="0" t="s">
+    <row r="34" spans="2:3">
+      <c r="B34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="36">
-      <c r="B36" s="0" t="s">
+    <row r="36" spans="2:3">
+      <c r="B36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="37">
-      <c r="B37" s="0" t="s">
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="38">
-      <c r="C38" s="0" t="s">
+    <row r="38" spans="2:3">
+      <c r="C38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="40">
-      <c r="B40" s="0" t="s">
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="41">
-      <c r="B41" s="0" t="s">
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="42">
-      <c r="B42" s="0" t="s">
+    <row r="42" spans="2:3">
+      <c r="B42" t="s">
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="44">
-      <c r="B44" s="0" t="s">
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="45">
-      <c r="B45" s="0" t="s">
+    <row r="45" spans="2:3">
+      <c r="B45" t="s">
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="47">
-      <c r="B47" s="0" t="s">
+    <row r="47" spans="2:3">
+      <c r="B47" t="s">
         <v>61</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="48">
-      <c r="C48" s="0" t="s">
+    <row r="48" spans="2:3">
+      <c r="C48" t="s">
         <v>62</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="49">
-      <c r="C49" s="0" t="s">
+    <row r="49" spans="1:5">
+      <c r="C49" t="s">
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="50">
-      <c r="D50" s="0" t="s">
+    <row r="50" spans="1:5">
+      <c r="D50" t="s">
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="51">
-      <c r="E51" s="0" t="s">
+    <row r="51" spans="1:5">
+      <c r="E51" t="s">
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="53">
-      <c r="C53" s="0" t="s">
+    <row r="53" spans="1:5">
+      <c r="C53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="54">
-      <c r="C54" s="0" t="s">
+    <row r="54" spans="1:5">
+      <c r="C54" t="s">
         <v>67</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="56">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="57">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="58">
-      <c r="B58" s="0" t="s">
+    <row r="58" spans="1:5">
+      <c r="B58" t="s">
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="59">
-      <c r="B59" s="0" t="s">
+    <row r="59" spans="1:5">
+      <c r="B59" t="s">
         <v>71</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="62">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
         <v>72</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="63">
-      <c r="B63" s="0" t="s">
+    <row r="63" spans="1:5">
+      <c r="B63" t="s">
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="64">
-      <c r="B64" s="0" t="s">
+    <row r="64" spans="1:5">
+      <c r="B64" t="s">
         <v>44</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="65">
-      <c r="B65" s="0" t="s">
+    <row r="65" spans="1:3">
+      <c r="B65" t="s">
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="66">
-      <c r="B66" s="0" t="s">
+    <row r="66" spans="1:3">
+      <c r="B66" t="s">
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="68">
-      <c r="B68" s="0" t="s">
+    <row r="68" spans="1:3">
+      <c r="B68" t="s">
         <v>75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="71">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="72">
-      <c r="B72" s="0" t="s">
+    <row r="72" spans="1:3">
+      <c r="B72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="73">
-      <c r="C73" s="0" t="s">
+    <row r="73" spans="1:3">
+      <c r="C73" t="s">
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="74">
-      <c r="C74" s="0" t="s">
+    <row r="74" spans="1:3">
+      <c r="C74" t="s">
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="75">
-      <c r="C75" s="0" t="s">
+    <row r="75" spans="1:3">
+      <c r="C75" t="s">
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="78">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="79">
-      <c r="B79" s="0" t="s">
+    <row r="79" spans="1:3">
+      <c r="B79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="80">
-      <c r="C80" s="0" t="s">
+    <row r="80" spans="1:3">
+      <c r="C80" t="s">
         <v>82</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="81">
-      <c r="C81" s="0" t="s">
+    <row r="81" spans="3:3">
+      <c r="C81" t="s">
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="82">
-      <c r="C82" s="0" t="s">
+    <row r="82" spans="3:3">
+      <c r="C82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="83">
-      <c r="C83" s="0" t="s">
+    <row r="83" spans="3:3">
+      <c r="C83" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A2:E130"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A76" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D102" activeCellId="0" pane="topLeft" sqref="D102"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
-      <c r="B2" s="0" t="s">
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
-      <c r="B3" s="0" t="s">
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
-      <c r="B5" s="0" t="s">
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
-      <c r="C6" s="0" t="s">
+    <row r="6" spans="2:4">
+      <c r="C6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
-      <c r="C7" s="0" t="s">
+    <row r="7" spans="2:4">
+      <c r="C7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
-      <c r="B9" s="0" t="s">
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
-      <c r="C10" s="0" t="s">
+    <row r="10" spans="2:4">
+      <c r="C10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="D11" s="0" t="s">
+    <row r="11" spans="2:4">
+      <c r="D11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
-      <c r="C13" s="0" t="s">
+    <row r="13" spans="2:4">
+      <c r="C13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
-      <c r="D14" s="0" t="s">
+    <row r="14" spans="2:4">
+      <c r="D14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="16">
-      <c r="C16" s="0" t="s">
+    <row r="16" spans="2:4">
+      <c r="C16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
-      <c r="D17" s="0" t="s">
+    <row r="17" spans="3:5">
+      <c r="D17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="18">
-      <c r="D18" s="0" t="s">
+    <row r="18" spans="3:5">
+      <c r="D18" t="s">
         <v>93</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="19">
-      <c r="E19" s="0" t="s">
+    <row r="19" spans="3:5">
+      <c r="E19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="21">
-      <c r="D21" s="0" t="s">
+    <row r="21" spans="3:5">
+      <c r="D21" t="s">
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="22">
-      <c r="E22" s="0" t="s">
+    <row r="22" spans="3:5">
+      <c r="E22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="23">
-      <c r="D23" s="0" t="s">
+    <row r="23" spans="3:5">
+      <c r="D23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
-      <c r="D24" s="0" t="s">
+    <row r="24" spans="3:5">
+      <c r="D24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
-      <c r="E25" s="0" t="s">
+    <row r="25" spans="3:5">
+      <c r="E25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
-      <c r="D27" s="0" t="s">
+    <row r="27" spans="3:5">
+      <c r="D27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="28">
-      <c r="E28" s="0" t="s">
+    <row r="28" spans="3:5">
+      <c r="E28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="30">
-      <c r="C30" s="0" t="s">
+    <row r="30" spans="3:5">
+      <c r="C30" t="s">
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="31">
-      <c r="D31" s="0" t="s">
+    <row r="31" spans="3:5">
+      <c r="D31" t="s">
         <v>101</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="32">
-      <c r="E32" s="0" t="s">
+    <row r="32" spans="3:5">
+      <c r="E32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="33">
-      <c r="E33" s="0" t="s">
+    <row r="33" spans="1:5">
+      <c r="E33" t="s">
         <v>102</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="35">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="36">
-      <c r="B36" s="0" t="s">
+    <row r="36" spans="1:5">
+      <c r="B36" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" t="s">
         <v>104</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="37">
-      <c r="B37" s="0" t="s">
+    <row r="37" spans="1:5">
+      <c r="B37" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="38">
-      <c r="B38" s="0" t="s">
+    <row r="38" spans="1:5">
+      <c r="B38" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" t="s">
         <v>108</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="39">
-      <c r="B39" s="0" t="s">
+    <row r="39" spans="1:5">
+      <c r="B39" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="40">
-      <c r="B40" s="0" t="s">
+    <row r="40" spans="1:5">
+      <c r="B40" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" t="s">
         <v>111</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="42">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="43">
-      <c r="B43" s="0" t="s">
+    <row r="43" spans="1:5">
+      <c r="B43" t="s">
         <v>112</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="44">
-      <c r="B44" s="0" t="s">
+    <row r="44" spans="1:5">
+      <c r="B44" t="s">
         <v>113</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="45">
-      <c r="B45" s="0" t="s">
+    <row r="45" spans="1:5">
+      <c r="B45" t="s">
         <v>114</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="46">
-      <c r="B46" s="0" t="s">
+    <row r="46" spans="1:5">
+      <c r="B46" t="s">
         <v>115</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="47">
-      <c r="B47" s="0" t="s">
+    <row r="47" spans="1:5">
+      <c r="B47" t="s">
         <v>116</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="49">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
         <v>117</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="50">
-      <c r="B50" s="0" t="s">
+    <row r="50" spans="1:3">
+      <c r="B50" t="s">
         <v>118</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="52">
-      <c r="B52" s="0" t="s">
+    <row r="52" spans="1:3">
+      <c r="B52" t="s">
         <v>117</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="53">
-      <c r="B53" s="0" t="s">
+    <row r="53" spans="1:3">
+      <c r="B53" t="s">
         <v>119</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="54">
-      <c r="B54" s="0" t="s">
+    <row r="54" spans="1:3">
+      <c r="B54" t="s">
         <v>120</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="55">
-      <c r="B55" s="0" t="s">
+    <row r="55" spans="1:3">
+      <c r="B55" t="s">
         <v>121</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="56">
-      <c r="C56" s="0" t="s">
+    <row r="56" spans="1:3">
+      <c r="C56" t="s">
         <v>122</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="58">
-      <c r="B58" s="0" t="s">
+    <row r="58" spans="1:3">
+      <c r="B58" t="s">
         <v>123</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="59">
-      <c r="B59" s="0" t="s">
+    <row r="59" spans="1:3">
+      <c r="B59" t="s">
         <v>124</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="61">
-      <c r="B61" s="0" t="s">
+    <row r="61" spans="1:3">
+      <c r="B61" t="s">
         <v>125</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="62">
-      <c r="C62" s="0" t="s">
+    <row r="62" spans="1:3">
+      <c r="C62" t="s">
         <v>126</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="63">
-      <c r="C63" s="0" t="s">
+    <row r="63" spans="1:3">
+      <c r="C63" t="s">
         <v>127</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="65">
-      <c r="B65" s="0" t="s">
+    <row r="65" spans="1:3">
+      <c r="B65" t="s">
         <v>128</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="66">
-      <c r="C66" s="0" t="s">
+    <row r="66" spans="1:3">
+      <c r="C66" t="s">
         <v>129</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="67">
-      <c r="C67" s="0" t="s">
+    <row r="67" spans="1:3">
+      <c r="C67" t="s">
         <v>130</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="68">
-      <c r="C68" s="0" t="s">
+    <row r="68" spans="1:3">
+      <c r="C68" t="s">
         <v>131</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="70">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
         <v>132</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="71">
-      <c r="B71" s="0" t="s">
+    <row r="71" spans="1:3">
+      <c r="B71" t="s">
         <v>133</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="72">
-      <c r="B72" s="0" t="s">
+    <row r="72" spans="1:3">
+      <c r="B72" t="s">
         <v>134</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="73">
-      <c r="B73" s="0" t="s">
+    <row r="73" spans="1:3">
+      <c r="B73" t="s">
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="74">
-      <c r="B74" s="0" t="s">
+    <row r="74" spans="1:3">
+      <c r="B74" t="s">
         <v>135</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="75">
-      <c r="B75" s="0" t="s">
+    <row r="75" spans="1:3">
+      <c r="B75" t="s">
         <v>136</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" t="s">
         <v>137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="77">
-      <c r="B77" s="0" t="s">
+    <row r="77" spans="1:3">
+      <c r="B77" t="s">
         <v>138</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="78">
-      <c r="B78" s="0" t="s">
+    <row r="78" spans="1:3">
+      <c r="B78" t="s">
         <v>139</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="79">
-      <c r="B79" s="0" t="s">
+    <row r="79" spans="1:3">
+      <c r="B79" t="s">
         <v>140</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="80">
-      <c r="B80" s="0" t="s">
+    <row r="80" spans="1:3">
+      <c r="B80" t="s">
         <v>141</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="82">
-      <c r="B82" s="0" t="s">
+    <row r="82" spans="1:2">
+      <c r="B82" t="s">
         <v>142</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="83">
-      <c r="B83" s="0" t="s">
+    <row r="83" spans="1:2">
+      <c r="B83" t="s">
         <v>143</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="86">
-      <c r="A86" s="0" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="87">
-      <c r="B87" s="0" t="s">
+    <row r="87" spans="1:2">
+      <c r="B87" t="s">
         <v>144</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="88">
-      <c r="B88" s="0" t="s">
+    <row r="88" spans="1:2">
+      <c r="B88" t="s">
         <v>145</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="89">
-      <c r="B89" s="0" t="s">
+    <row r="89" spans="1:2">
+      <c r="B89" t="s">
         <v>146</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="90">
-      <c r="B90" s="0" t="s">
+    <row r="90" spans="1:2">
+      <c r="B90" t="s">
         <v>147</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="91">
-      <c r="B91" s="0" t="s">
+    <row r="91" spans="1:2">
+      <c r="B91" t="s">
         <v>148</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="92">
-      <c r="B92" s="0" t="s">
+    <row r="92" spans="1:2">
+      <c r="B92" t="s">
         <v>149</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="94">
-      <c r="B94" s="0" t="s">
+    <row r="94" spans="1:2">
+      <c r="B94" t="s">
         <v>150</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="97">
-      <c r="A97" s="0" t="s">
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
         <v>151</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="98">
-      <c r="B98" s="0" t="s">
+    <row r="98" spans="1:3">
+      <c r="B98" t="s">
         <v>152</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="99">
-      <c r="C99" s="0" t="s">
+    <row r="99" spans="1:3">
+      <c r="C99" t="s">
         <v>153</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="100">
-      <c r="C100" s="0" t="s">
+    <row r="100" spans="1:3">
+      <c r="C100" t="s">
         <v>154</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="101">
-      <c r="B101" s="0" t="s">
+    <row r="101" spans="1:3">
+      <c r="B101" t="s">
         <v>155</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="103">
-      <c r="B103" s="0" t="s">
+    <row r="103" spans="1:3">
+      <c r="B103" t="s">
         <v>152</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="104">
-      <c r="C104" s="0" t="s">
+    <row r="104" spans="1:3">
+      <c r="C104" t="s">
         <v>153</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="105">
-      <c r="C105" s="0" t="s">
+    <row r="105" spans="1:3">
+      <c r="C105" t="s">
         <v>156</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="106">
-      <c r="B106" s="0" t="s">
+    <row r="106" spans="1:3">
+      <c r="B106" t="s">
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="108">
-      <c r="B108" s="0" t="s">
+    <row r="108" spans="1:3">
+      <c r="B108" t="s">
         <v>152</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="109">
-      <c r="C109" s="0" t="s">
+    <row r="109" spans="1:3">
+      <c r="C109" t="s">
         <v>153</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="110">
-      <c r="C110" s="0" t="s">
+    <row r="110" spans="1:3">
+      <c r="C110" t="s">
         <v>158</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="111">
-      <c r="B111" s="0" t="s">
+    <row r="111" spans="1:3">
+      <c r="B111" t="s">
         <v>159</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="112">
-      <c r="B112" s="0" t="s">
+    <row r="112" spans="1:3">
+      <c r="B112" t="s">
         <v>160</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="114">
-      <c r="A114" s="0" t="s">
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
         <v>161</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="115">
-      <c r="A115" s="0" t="s">
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
         <v>162</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="116">
-      <c r="A116" s="0" t="s">
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
         <v>163</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="117">
-      <c r="A117" s="0" t="s">
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
         <v>164</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="118">
-      <c r="A118" s="0" t="s">
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
         <v>165</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="119">
-      <c r="A119" s="0" t="s">
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
         <v>166</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="120">
-      <c r="A120" s="0" t="s">
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
         <v>167</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="121">
-      <c r="A121" s="0" t="s">
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
         <v>168</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="124">
-      <c r="A124" s="0" t="s">
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="125">
-      <c r="B125" s="0" t="s">
+    <row r="125" spans="1:2">
+      <c r="B125" t="s">
         <v>169</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="127">
-      <c r="A127" s="0" t="s">
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="128">
-      <c r="B128" s="0" t="s">
+    <row r="128" spans="1:2">
+      <c r="B128" t="s">
         <v>170</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="129">
-      <c r="B129" s="0" t="s">
+    <row r="129" spans="2:2">
+      <c r="B129" t="s">
         <v>171</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="130">
-      <c r="B130" s="0" t="s">
+    <row r="130" spans="2:2">
+      <c r="B130" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A27" activeCellId="0" pane="topLeft" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
-      <c r="B4" s="0" t="s">
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
-      <c r="B5" s="0" t="s">
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
-      <c r="B6" s="0" t="s">
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
         <v>177</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
-      <c r="C7" s="0" t="s">
+    <row r="7" spans="1:3">
+      <c r="C7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
-      <c r="C8" s="0" t="s">
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="9">
-      <c r="C9" s="0" t="s">
+    <row r="9" spans="1:3">
+      <c r="C9" t="s">
         <v>180</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
-      <c r="C10" s="0" t="s">
+    <row r="10" spans="1:3">
+      <c r="C10" t="s">
         <v>181</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="C11" s="0" t="s">
+    <row r="11" spans="1:3">
+      <c r="C11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
-      <c r="B13" s="0" t="s">
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
         <v>183</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="14">
-      <c r="B14" s="0" t="s">
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="16">
-      <c r="B16" s="0" t="s">
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="17">
+    <row r="17" spans="1:3">
       <c r="A17" s="1"/>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>186</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="20">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="21">
+    <row r="21" spans="1:3">
       <c r="A21" s="2"/>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2"/>
+      <c r="B22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2"/>
+      <c r="B23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="22">
-      <c r="A22" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="23">
-      <c r="A23" s="2"/>
-      <c r="B23" s="0" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2"/>
+      <c r="B25" t="s">
         <v>189</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
-      <c r="B24" s="0" t="s">
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
         <v>190</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="25">
-      <c r="C25" s="0" t="s">
+    <row r="27" spans="1:3">
+      <c r="C27" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1"/>
+      <c r="B28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="B33" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="B34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="B35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="B36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="B37" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="B43" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
         <v>191</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="26">
-      <c r="A26" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
-      <c r="A27" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="30">
-      <c r="A30" s="0" t="s">
+    <row r="47" spans="1:2">
+      <c r="B47" t="s">
         <v>192</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="31">
-      <c r="B31" s="0" t="s">
+    <row r="48" spans="1:2">
+      <c r="B48" t="s">
         <v>193</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="32">
-      <c r="B32" s="0" t="s">
+    <row r="49" spans="1:9">
+      <c r="B49" t="s">
         <v>194</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="33">
-      <c r="B33" s="0" t="s">
+    <row r="50" spans="1:9">
+      <c r="B50" t="s">
         <v>195</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="34">
-      <c r="B34" s="0" t="s">
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="37">
-      <c r="A37" s="0" t="s">
+      <c r="I53" t="s">
         <v>197</v>
       </c>
-      <c r="I37" s="0" t="s">
+    </row>
+    <row r="54" spans="1:9">
+      <c r="B54" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="38">
-      <c r="B38" s="0" t="s">
+      <c r="I54" t="s">
         <v>199</v>
       </c>
-      <c r="I38" s="0" t="s">
+    </row>
+    <row r="55" spans="1:9">
+      <c r="B55" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="39">
-      <c r="B39" s="0" t="s">
+      <c r="I55" t="s">
         <v>201</v>
       </c>
-      <c r="I39" s="0" t="s">
+    </row>
+    <row r="56" spans="1:9">
+      <c r="B56" t="s">
         <v>202</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="40">
-      <c r="B40" s="0" t="s">
+    <row r="57" spans="1:9">
+      <c r="C57" t="s">
         <v>203</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="41">
-      <c r="C41" s="0" t="s">
+    <row r="58" spans="1:9">
+      <c r="C58" t="s">
         <v>204</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="42">
-      <c r="C42" s="0" t="s">
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
         <v>205</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="44">
-      <c r="A44" s="0" t="s">
+    <row r="65" spans="1:2">
+      <c r="B65" t="s">
         <v>206</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="45">
-      <c r="B45" s="0" t="s">
+    <row r="66" spans="1:2">
+      <c r="B66" t="s">
         <v>207</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="48">
-      <c r="A48" s="0" t="s">
+    <row r="67" spans="1:2">
+      <c r="B67" t="s">
         <v>208</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="49">
-      <c r="B49" s="0" t="s">
+    <row r="68" spans="1:2">
+      <c r="B68" t="s">
         <v>209</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="50">
-      <c r="B50" s="0" t="s">
+    <row r="69" spans="1:2">
+      <c r="B69" t="s">
         <v>210</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="51">
-      <c r="B51" s="0" t="s">
+    <row r="70" spans="1:2">
+      <c r="B70" t="s">
         <v>211</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="52">
-      <c r="B52" s="0" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
         <v>212</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="53">
-      <c r="B53" s="0" t="s">
+    <row r="74" spans="1:2">
+      <c r="B74" t="s">
         <v>213</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="54">
-      <c r="B54" s="0" t="s">
+    <row r="75" spans="1:2">
+      <c r="B75" t="s">
         <v>214</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="57">
-      <c r="A57" s="0" t="s">
+    <row r="76" spans="1:2">
+      <c r="B76" t="s">
         <v>215</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="58">
-      <c r="B58" s="0" t="s">
+    <row r="77" spans="1:2">
+      <c r="B77" t="s">
         <v>216</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="59">
-      <c r="B59" s="0" t="s">
+    <row r="78" spans="1:2">
+      <c r="B78" t="s">
         <v>217</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="60">
-      <c r="B60" s="0" t="s">
+    <row r="79" spans="1:2">
+      <c r="B79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="61">
-      <c r="B61" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="62">
-      <c r="B62" s="0" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="63">
-      <c r="B63" s="0" t="s">
-        <v>221</v>
-      </c>
-    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>